<commit_message>
Add captions to supp tables
</commit_message>
<xml_diff>
--- a/supp_tables.xlsx
+++ b/supp_tables.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wickr/Library/CloudStorage/Dropbox/Uni_research/Projects/2024-01_low-depth_Illumina_polishing/depth_vs_polishing_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wickr/Library/CloudStorage/Dropbox/Uni_research/Projects/2024-01_low-depth_polishing_paper/depth_vs_polishing_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43528DD4-C365-0248-B35E-F43CB3D90768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9058DA-1D50-0241-A290-3B2AA31C2D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="-18660" windowWidth="28040" windowHeight="17120" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
+    <workbookView xWindow="2940" yWindow="-21100" windowWidth="28040" windowHeight="17120" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Accessions" sheetId="2" r:id="rId1"/>
-    <sheet name="Medaka polishing" sheetId="1" r:id="rId2"/>
+    <sheet name="Table S1, accessions" sheetId="2" r:id="rId1"/>
+    <sheet name="Table S2, Medaka polishing" sheetId="1" r:id="rId2"/>
+    <sheet name="Table S3, Better or worse" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>Genome</t>
   </si>
@@ -178,7 +179,109 @@
     <t>SAMN38321311</t>
   </si>
   <si>
-    <t>Of the nine ONT-only assemblies used in this study, three improved with Medaka polishing, three did not change, three got worse, and Medaka made the total error count worse. We therefore do not recommend using Medaka to polish Trycycler assemblies of sup-basecalled ONT reads.</t>
+    <t>HyPo</t>
+  </si>
+  <si>
+    <t>FMLRC2</t>
+  </si>
+  <si>
+    <t>NextPolish</t>
+  </si>
+  <si>
+    <t>Pilon</t>
+  </si>
+  <si>
+    <t>Polypolish default</t>
+  </si>
+  <si>
+    <t>Polypolish careful</t>
+  </si>
+  <si>
+    <t>Pypolca default</t>
+  </si>
+  <si>
+    <t>Pypolca careful</t>
+  </si>
+  <si>
+    <t>Better</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>Worse</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table S3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Each polisher was run 4500 times (9 genomes at 500 depths). Each result was classified as 'Better' (fewer errors after polishing), 'Same' (no change in errors after polishing) or 'Worse' (more errors after polishing), with the totals shown in this table.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table S1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: NCBI accessions for each of the nine genomes used in this study and their ONT and Illumina read sets.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table S2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Of the nine ONT-only assemblies used in this study, three improved with Medaka polishing (blue), three did not change, three got worse (red), and Medaka made the total error count worse. We therefore do not recommend using Medaka to polish Trycycler assemblies of sup-basecalled ONT reads.</t>
+    </r>
+  </si>
+  <si>
+    <t>Polisher</t>
   </si>
 </sst>
 </file>
@@ -186,7 +289,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -214,13 +317,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFCD6D6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -255,42 +358,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -298,13 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -313,7 +384,7 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -321,21 +392,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -343,6 +438,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFCD6D6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -355,9 +455,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -395,7 +495,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -501,7 +601,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -643,7 +743,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -651,11 +751,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329A5B2C-B2CD-2E4C-9B25-8D30DFCCCE6A}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -666,146 +764,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="5" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="12" spans="1:4" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A12:D12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -815,281 +924,281 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="4" customWidth="1"/>
     <col min="6" max="6" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="3">
         <v>1768448</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="4">
         <v>5</v>
       </c>
-      <c r="D3" s="10" t="str">
+      <c r="D3" s="2" t="str">
         <f>CONCATENATE("Q", IF(C3=0, "∞", ROUND(-10*LOG10(C3/$B3), 1)))</f>
         <v>Q55.5</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="25">
         <v>3</v>
       </c>
-      <c r="F3" s="12" t="str">
+      <c r="F3" s="26" t="str">
         <f>CONCATENATE("Q", IF(E3=0, "∞", ROUND(-10*LOG10(E3/$B3), 1)))</f>
         <v>Q57.7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="3">
         <v>1513368</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="4">
         <v>18</v>
       </c>
-      <c r="D4" s="10" t="str">
+      <c r="D4" s="2" t="str">
         <f t="shared" ref="D4:F12" si="0">CONCATENATE("Q", IF(C4=0, "∞", ROUND(-10*LOG10(C4/$B4), 1)))</f>
         <v>Q49.2</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="21">
         <v>28</v>
       </c>
-      <c r="F4" s="14" t="str">
+      <c r="F4" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Q47.3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="3">
         <v>5204893</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="str">
+      <c r="D5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Q67.2</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="10" t="str">
+      <c r="F5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Q67.2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="3">
         <v>2919549</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="4">
         <v>5</v>
       </c>
-      <c r="D6" s="10" t="str">
+      <c r="D6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Q57.7</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="25">
         <v>4</v>
       </c>
-      <c r="F6" s="12" t="str">
+      <c r="F6" s="26" t="str">
         <f t="shared" si="0"/>
         <v>Q58.6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="3">
         <v>2944530</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="4">
         <v>0</v>
       </c>
-      <c r="D7" s="10" t="str">
+      <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Q∞</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="4">
         <v>0</v>
       </c>
-      <c r="F7" s="10" t="str">
+      <c r="F7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Q∞</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="3">
         <v>2814137</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="4">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="str">
+      <c r="D8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Q64.5</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="4">
         <v>1</v>
       </c>
-      <c r="F8" s="10" t="str">
+      <c r="F8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Q64.5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="3">
         <v>4801704</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="4">
         <v>3</v>
       </c>
-      <c r="D9" s="10" t="str">
+      <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Q62</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="21">
         <v>6</v>
       </c>
-      <c r="F9" s="14" t="str">
+      <c r="F9" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Q59</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="3">
         <v>4142374</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="4">
         <v>2</v>
       </c>
-      <c r="D10" s="10" t="str">
+      <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Q63.2</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="21">
         <v>3</v>
       </c>
-      <c r="F10" s="14" t="str">
+      <c r="F10" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Q61.4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="13">
         <v>5147091</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="14">
         <v>2</v>
       </c>
-      <c r="D11" s="27" t="str">
+      <c r="D11" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Q64.1</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="27">
         <v>1</v>
       </c>
-      <c r="F11" s="29" t="str">
+      <c r="F11" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Q67.1</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="6">
         <f>SUM(B3:B11)</f>
         <v>31256094</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="7">
         <f>SUM(C3:C11)</f>
         <v>37</v>
       </c>
-      <c r="D12" s="18" t="str">
+      <c r="D12" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Q59.3</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="23">
         <f>SUM(E3:E11)</f>
         <v>47</v>
       </c>
-      <c r="F12" s="20" t="str">
+      <c r="F12" s="24" t="str">
         <f t="shared" si="0"/>
         <v>Q58.2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
+    <row r="14" spans="1:6" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1099,7 +1208,163 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D12:D13" formula="1"/>
+    <ignoredError sqref="D12:D13 E12" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EE2DF7-98EF-4249-A1FC-51F4F86D2B9C}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>3260</v>
+      </c>
+      <c r="C2">
+        <v>1093</v>
+      </c>
+      <c r="D2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>3321</v>
+      </c>
+      <c r="C3">
+        <v>1179</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>2656</v>
+      </c>
+      <c r="C4">
+        <v>470</v>
+      </c>
+      <c r="D4">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>3526</v>
+      </c>
+      <c r="C5">
+        <v>923</v>
+      </c>
+      <c r="D5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>1007</v>
+      </c>
+      <c r="C6">
+        <v>396</v>
+      </c>
+      <c r="D6">
+        <v>3097</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>1450</v>
+      </c>
+      <c r="C7">
+        <v>379</v>
+      </c>
+      <c r="D7">
+        <v>2671</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <v>1851</v>
+      </c>
+      <c r="C8">
+        <v>460</v>
+      </c>
+      <c r="D8">
+        <v>2189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2462</v>
+      </c>
+      <c r="C9" s="5">
+        <v>707</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:D11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some more changes to supp tables
</commit_message>
<xml_diff>
--- a/supp_tables.xlsx
+++ b/supp_tables.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wickr/Library/CloudStorage/Dropbox/Uni_research/Projects/2024-01_low-depth_polishing_paper/depth_vs_polishing_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1667917/Documents/Wick/depth_vs_polishing_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9058DA-1D50-0241-A290-3B2AA31C2D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1CF6C6-FFCB-0F48-AC3A-DC6681A624C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="-21100" windowWidth="28040" windowHeight="17120" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17980" activeTab="3" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1, accessions" sheetId="2" r:id="rId1"/>
     <sheet name="Table S2, Medaka polishing" sheetId="1" r:id="rId2"/>
-    <sheet name="Table S3, Better or worse" sheetId="3" r:id="rId3"/>
+    <sheet name="Table S3, Single &gt;25x" sheetId="5" r:id="rId3"/>
+    <sheet name="Table S4, Combination &gt;25x" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
   <si>
     <t>Genome</t>
   </si>
@@ -185,9 +186,6 @@
     <t>FMLRC2</t>
   </si>
   <si>
-    <t>NextPolish</t>
-  </si>
-  <si>
     <t>Pilon</t>
   </si>
   <si>
@@ -203,36 +201,7 @@
     <t>Pypolca careful</t>
   </si>
   <si>
-    <t>Better</t>
-  </si>
-  <si>
-    <t>Same</t>
-  </si>
-  <si>
     <t>Worse</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Table S3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Each polisher was run 4500 times (9 genomes at 500 depths). Each result was classified as 'Better' (fewer errors after polishing), 'Same' (no change in errors after polishing) or 'Worse' (more errors after polishing), with the totals shown in this table.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -281,7 +250,76 @@
     </r>
   </si>
   <si>
-    <t>Polisher</t>
+    <t xml:space="preserve">First Polisher  </t>
+  </si>
+  <si>
+    <t>Second Polisher</t>
+  </si>
+  <si>
+    <t>Mean Errors</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard Deviation </t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>No Worse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polisher  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NextPolish </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Table S3: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Summary Statistics of Remaining Errors for Single Polishers at All Depth Intervals from 25.0× to 50.0× (251 Samples)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Table S4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Summary Statistics of Remaining Errors for Sequential Polishers at All Depth Intervals from 25.0× to 50.0× (251 Samples)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -291,7 +329,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -306,6 +344,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -358,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -399,38 +450,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,9 +512,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -495,7 +552,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -601,7 +658,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -743,7 +800,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -753,7 +810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329A5B2C-B2CD-2E4C-9B25-8D30DFCCCE6A}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -904,12 +961,12 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="A12" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -924,7 +981,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -938,14 +995,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="18"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -981,10 +1038,10 @@
         <f>CONCATENATE("Q", IF(C3=0, "∞", ROUND(-10*LOG10(C3/$B3), 1)))</f>
         <v>Q55.5</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="22">
         <v>3</v>
       </c>
-      <c r="F3" s="26" t="str">
+      <c r="F3" s="23" t="str">
         <f>CONCATENATE("Q", IF(E3=0, "∞", ROUND(-10*LOG10(E3/$B3), 1)))</f>
         <v>Q57.7</v>
       </c>
@@ -1003,10 +1060,10 @@
         <f t="shared" ref="D4:F12" si="0">CONCATENATE("Q", IF(C4=0, "∞", ROUND(-10*LOG10(C4/$B4), 1)))</f>
         <v>Q49.2</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="18">
         <v>28</v>
       </c>
-      <c r="F4" s="22" t="str">
+      <c r="F4" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Q47.3</v>
       </c>
@@ -1047,10 +1104,10 @@
         <f t="shared" si="0"/>
         <v>Q57.7</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <v>4</v>
       </c>
-      <c r="F6" s="26" t="str">
+      <c r="F6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>Q58.6</v>
       </c>
@@ -1113,10 +1170,10 @@
         <f t="shared" si="0"/>
         <v>Q62</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="18">
         <v>6</v>
       </c>
-      <c r="F9" s="22" t="str">
+      <c r="F9" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Q59</v>
       </c>
@@ -1135,10 +1192,10 @@
         <f t="shared" si="0"/>
         <v>Q63.2</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="18">
         <v>3</v>
       </c>
-      <c r="F10" s="22" t="str">
+      <c r="F10" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Q61.4</v>
       </c>
@@ -1157,10 +1214,10 @@
         <f t="shared" si="0"/>
         <v>Q64.1</v>
       </c>
-      <c r="E11" s="27">
-        <v>1</v>
-      </c>
-      <c r="F11" s="28" t="str">
+      <c r="E11" s="24">
+        <v>1</v>
+      </c>
+      <c r="F11" s="25" t="str">
         <f t="shared" si="0"/>
         <v>Q67.1</v>
       </c>
@@ -1181,24 +1238,24 @@
         <f t="shared" si="0"/>
         <v>Q59.3</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="20">
         <f>SUM(E3:E11)</f>
         <v>47</v>
       </c>
-      <c r="F12" s="24" t="str">
+      <c r="F12" s="21" t="str">
         <f t="shared" si="0"/>
         <v>Q58.2</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="A14" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1214,156 +1271,554 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9EE2DF7-98EF-4249-A1FC-51F4F86D2B9C}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2A52BF-89B5-F84A-9572-1BEA1D441973}">
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A13" sqref="A13:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="E3" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>30.22</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>38.619999999999997</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>246</v>
+      </c>
+      <c r="G4">
+        <v>190</v>
+      </c>
+      <c r="H4">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>28.22</v>
+      </c>
+      <c r="C5">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>9.82</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>68</v>
+      </c>
+      <c r="G5">
+        <v>211</v>
+      </c>
+      <c r="H5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6">
+        <v>8.4</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>6.24</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>34</v>
+      </c>
+      <c r="G6">
+        <v>251</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>65.53</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>132.02000000000001</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>953</v>
+      </c>
+      <c r="G7">
+        <v>185</v>
+      </c>
+      <c r="H7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8">
+        <v>7.16</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>2.35</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>251</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>50</v>
       </c>
-      <c r="B2">
-        <v>3260</v>
-      </c>
-      <c r="C2">
-        <v>1093</v>
-      </c>
-      <c r="D2">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B9">
+        <v>7.3</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>251</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>51</v>
       </c>
-      <c r="B3">
-        <v>3321</v>
-      </c>
-      <c r="C3">
-        <v>1179</v>
-      </c>
-      <c r="D3">
+      <c r="B10">
+        <v>2.13</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2.15</v>
+      </c>
+      <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="F10">
+        <v>28</v>
+      </c>
+      <c r="G10">
+        <v>251</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B4">
-        <v>2656</v>
-      </c>
-      <c r="C4">
-        <v>470</v>
-      </c>
-      <c r="D4">
-        <v>1374</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5">
-        <v>3526</v>
-      </c>
-      <c r="C5">
-        <v>923</v>
-      </c>
-      <c r="D5">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6">
-        <v>1007</v>
-      </c>
-      <c r="C6">
-        <v>396</v>
-      </c>
-      <c r="D6">
-        <v>3097</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7">
-        <v>1450</v>
-      </c>
-      <c r="C7">
-        <v>379</v>
-      </c>
-      <c r="D7">
-        <v>2671</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8">
-        <v>1851</v>
-      </c>
-      <c r="C8">
-        <v>460</v>
-      </c>
-      <c r="D8">
-        <v>2189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="5">
-        <v>2462</v>
-      </c>
-      <c r="C9" s="5">
-        <v>707</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="104" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
+      <c r="B11" s="5">
+        <v>1.62</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.05</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>6</v>
+      </c>
+      <c r="G11" s="5">
+        <v>251</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A13:J13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF30A77-3566-8C4B-92CC-3F903D073C1A}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3">
+        <v>1.62</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1.06</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>2.13</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2.15</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>28</v>
+      </c>
+      <c r="H4">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>1.64</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1.07</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <v>2.14</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2.16</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>28</v>
+      </c>
+      <c r="H6">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>1.62</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1.06</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>1.65</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1.08</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>2.13</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2.15</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>28</v>
+      </c>
+      <c r="H9">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2.15</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2.16</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>28</v>
+      </c>
+      <c r="H10" s="5">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Edit supp tables and parameter sweep
</commit_message>
<xml_diff>
--- a/supp_tables.xlsx
+++ b/supp_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wickr/Library/CloudStorage/Dropbox/Uni_research/Projects/2024-01_low-depth_polishing_paper/depth_vs_polishing_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1594C03-1750-7F48-A416-7BFB4A7E3F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9444A9C-42B6-5747-94B6-D7FE2ACCC6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12180" yWindow="-24260" windowWidth="30240" windowHeight="17180" activeTab="4" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
+    <workbookView xWindow="-360" yWindow="-26200" windowWidth="30240" windowHeight="17180" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1, accessions" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="100">
   <si>
     <t>Genome</t>
   </si>
@@ -89,9 +89,6 @@
   <si>
     <t>Trycycler+
 Medaka</t>
-  </si>
-  <si>
-    <t>ONT reads</t>
   </si>
   <si>
     <t>Illumina reads</t>
@@ -216,6 +213,111 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">First Polisher  </t>
+  </si>
+  <si>
+    <t>Second Polisher</t>
+  </si>
+  <si>
+    <t>Mean Errors</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard Deviation </t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>No Worse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polisher  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NextPolish </t>
+  </si>
+  <si>
+    <t>Polypolish-default</t>
+  </si>
+  <si>
+    <t>Polypolish-careful</t>
+  </si>
+  <si>
+    <t>Pypolca-default</t>
+  </si>
+  <si>
+    <t>Pypolca-careful</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Default parameters</t>
+  </si>
+  <si>
+    <t>Total errors (default parameters)</t>
+  </si>
+  <si>
+    <t>Best parameters</t>
+  </si>
+  <si>
+    <t>Total errors (best parameters)</t>
+  </si>
+  <si>
+    <t>Total errors (worst parameters)</t>
+  </si>
+  <si>
+    <t>-k 21 59 -m 5 -f 0.1</t>
+  </si>
+  <si>
+    <t>-k 27 -m 0 -f 0.29</t>
+  </si>
+  <si>
+    <t>-m 5 -x -4 -g -8 -n 20 -q 2</t>
+  </si>
+  <si>
+    <t>-m 5 -x -5 -g -8 -n 20 -q 41</t>
+  </si>
+  <si>
+    <t>NextPolish</t>
+  </si>
+  <si>
+    <t>-min_map_quality 0 -max_ins_fold_sgs 5 -max_clip_ratio_sgs 0.15 -trim_len_edge 2 -ext_len_edge 2 -indel_balance_factor_sgs 0.5 -min_count_ratio_skip 0.8 -max_len_kmer 50 -min_len_inter_kmer 5 -max_count_kmer 50</t>
+  </si>
+  <si>
+    <t>-min_map_quality 1 -max_ins_fold_sgs 7 -max_clip_ratio_sgs 0 -trim_len_edge 0 -ext_len_edge 0 -indel_balance_factor_sgs 0.63 -min_count_ratio_skip 0.55 -max_len_kmer 35 -min_len_inter_kmer 5 -max_count_kmer 47</t>
+  </si>
+  <si>
+    <t>--fix all --flank 10 --K 47 --mindepth 0.1 --minmq 0 --minqual 0</t>
+  </si>
+  <si>
+    <t>--fix bases --flank 3 --K 51 --mindepth 3 --minmq 58 --minqual 15</t>
+  </si>
+  <si>
+    <t>Polypolish</t>
+  </si>
+  <si>
+    <t>-i 0.2 -v 0.5 -m 10 -d 5</t>
+  </si>
+  <si>
+    <t>-i 0.42 -v 0.68 -m 3 -d 3</t>
+  </si>
+  <si>
+    <t>Pypolca</t>
+  </si>
+  <si>
+    <t>--min_alt 2 --min_ratio 2.0</t>
+  </si>
+  <si>
+    <t>--min_alt 3 --min_ratio 3.01</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -223,9 +325,8 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>Table S2</t>
+      <t xml:space="preserve">Table S3: </t>
     </r>
     <r>
       <rPr>
@@ -233,40 +334,9 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>: Of the nine ONT-only assemblies used in this study, three improved with Medaka polishing (blue), three did not change, three got worse (red), and Medaka made the total error count worse. We therefore do not recommend using Medaka to polish Trycycler assemblies of sup-basecalled ONT reads.</t>
+      <t>Summary statistics of remaining errors for single polishers at all depth intervals from 25.0× to 50.0× (251 samples).</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">First Polisher  </t>
-  </si>
-  <si>
-    <t>Second Polisher</t>
-  </si>
-  <si>
-    <t>Mean Errors</t>
-  </si>
-  <si>
-    <t>Median</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard Deviation </t>
-  </si>
-  <si>
-    <t>Minimum</t>
-  </si>
-  <si>
-    <t>Maximum</t>
-  </si>
-  <si>
-    <t>No Worse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polisher  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NextPolish </t>
   </si>
   <si>
     <r>
@@ -274,29 +344,8 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Table S3: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Summary Statistics of Remaining Errors for Single Polishers at All Depth Intervals from 25.0× to 50.0× (251 Samples)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Table S4:</t>
     </r>
@@ -304,86 +353,11 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Summary Statistics of Remaining Errors for Sequential Polishers at All Depth Intervals from 25.0× to 50.0× (251 Samples)</t>
+      <t xml:space="preserve"> Summary statistics of remaining errors for sequential polishers at all depth intervals from 25.0× to 50.0× (251 samples).</t>
     </r>
-  </si>
-  <si>
-    <t>Polypolish-default</t>
-  </si>
-  <si>
-    <t>Polypolish-careful</t>
-  </si>
-  <si>
-    <t>Pypolca-default</t>
-  </si>
-  <si>
-    <t>Pypolca-careful</t>
-  </si>
-  <si>
-    <t>Tool</t>
-  </si>
-  <si>
-    <t>Default parameters</t>
-  </si>
-  <si>
-    <t>Total errors (default parameters)</t>
-  </si>
-  <si>
-    <t>Best parameters</t>
-  </si>
-  <si>
-    <t>Total errors (best parameters)</t>
-  </si>
-  <si>
-    <t>Total errors (worst parameters)</t>
-  </si>
-  <si>
-    <t>-k 21 59 -m 5 -f 0.1</t>
-  </si>
-  <si>
-    <t>-k 27 -m 0 -f 0.29</t>
-  </si>
-  <si>
-    <t>-m 5 -x -4 -g -8 -n 20 -q 2</t>
-  </si>
-  <si>
-    <t>-m 5 -x -5 -g -8 -n 20 -q 41</t>
-  </si>
-  <si>
-    <t>NextPolish</t>
-  </si>
-  <si>
-    <t>-min_map_quality 0 -max_ins_fold_sgs 5 -max_clip_ratio_sgs 0.15 -trim_len_edge 2 -ext_len_edge 2 -indel_balance_factor_sgs 0.5 -min_count_ratio_skip 0.8 -max_len_kmer 50 -min_len_inter_kmer 5 -max_count_kmer 50</t>
-  </si>
-  <si>
-    <t>-min_map_quality 1 -max_ins_fold_sgs 7 -max_clip_ratio_sgs 0 -trim_len_edge 0 -ext_len_edge 0 -indel_balance_factor_sgs 0.63 -min_count_ratio_skip 0.55 -max_len_kmer 35 -min_len_inter_kmer 5 -max_count_kmer 47</t>
-  </si>
-  <si>
-    <t>--fix all --flank 10 --K 47 --mindepth 0.1 --minmq 0 --minqual 0</t>
-  </si>
-  <si>
-    <t>--fix bases --flank 3 --K 51 --mindepth 3 --minmq 58 --minqual 15</t>
-  </si>
-  <si>
-    <t>Polypolish</t>
-  </si>
-  <si>
-    <t>-i 0.2 -v 0.5 -m 10 -d 5</t>
-  </si>
-  <si>
-    <t>-i 0.42 -v 0.68 -m 3 -d 3</t>
-  </si>
-  <si>
-    <t>Pypolca</t>
-  </si>
-  <si>
-    <t>--min_alt 2 --min_ratio 2.0</t>
-  </si>
-  <si>
-    <t>--min_alt 3 --min_ratio 3.01</t>
   </si>
   <si>
     <r>
@@ -405,7 +379,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: for each polishing tool, we did a sweep to find the best parameter set for low-depth polishing. We used the </t>
+      <t xml:space="preserve">: Low-depth polishing parameter sweep.
+For each polishing tool, we did a sweep to find the best parameter set for low-depth polishing. We used the </t>
     </r>
     <r>
       <rPr>
@@ -426,8 +401,67 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> genome because it had the highest error count of our input genomes (18 errors) and tested 5x, 10x, 15x and 20x read depth. For each tool, we tried 1000 different sets of parameters which included both random choices and mutated versions of the best-performing parameter set.</t>
+      <t xml:space="preserve"> genome because it had the highest error count of our input genomes (18 errors) and tested 5x, 10x, 15x and 20x read depth. The reported error counts are the sum of errors at these four depths, so values below 72 indicate a net improvement in accuracy and values above 72 indicate a net reduction in accuracy. For each tool, we tried 1000 different sets of parameters which included both random choices and mutated versions of the best-performing parameter set.
+FMLRC2 and Pilon had the largest relative decrease in total errors, i.e. they benefitted the most from parameter tuning for low-depth polishing. HyPo had the smallest relative decrease in total errors, i.e. it benefitted the least from parameter tuning. While NextPolish could be tuned to have 38% fewer errors than its default settings, it still performed poorly at 5x depth, leading to a large total error count.
+Pypolca performed the best with tuned parameters, achieving 11 errors at 5x depth, 3 errors at 10x depth, 0 errors at 15x depth and 0 errors at 20x depth. Pypolca's tuned parameters were in between its default parameters and those used by its --careful option.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table S2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Medaka-polishing results.
+Of the nine ONT-only assemblies used in this study, three improved with Medaka polishing (blue), three did not change, three got worse (red), and Medaka made the total error count worse. We therefore do not recommend using Medaka to polish Trycycler assemblies of sup-basecalled ONT reads.</t>
+    </r>
+  </si>
+  <si>
+    <t>ONT reads (main analysis)</t>
+  </si>
+  <si>
+    <t>ONT reads (low-quality drafts)</t>
+  </si>
+  <si>
+    <t>SRR26899119</t>
+  </si>
+  <si>
+    <t>SRR26899114</t>
+  </si>
+  <si>
+    <t>SRR26899127</t>
+  </si>
+  <si>
+    <t>SRR26899134</t>
+  </si>
+  <si>
+    <t>SRR26899100</t>
+  </si>
+  <si>
+    <t>SRR26899108</t>
+  </si>
+  <si>
+    <t>SRR26899124</t>
+  </si>
+  <si>
+    <t>SRR26899094</t>
+  </si>
+  <si>
+    <t>SRR26899140</t>
   </si>
 </sst>
 </file>
@@ -454,25 +488,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -525,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -590,13 +624,28 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -605,25 +654,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -945,171 +976,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329A5B2C-B2CD-2E4C-9B25-8D30DFCCCE6A}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
+    </row>
+    <row r="12" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1120,7 +1180,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:F14"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1134,14 +1194,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="29"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1386,15 +1446,15 @@
         <v>Q58.2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
+    <row r="14" spans="1:6" ht="110" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1411,7 +1471,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2A52BF-89B5-F84A-9572-1BEA1D441973}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -1420,115 +1480,163 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="16" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="G1" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>49</v>
+      <c r="H1" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>30.22</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>38.619999999999997</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>246</v>
+      </c>
+      <c r="G2">
+        <v>190</v>
+      </c>
+      <c r="H2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>28.22</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>9.82</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>68</v>
+      </c>
+      <c r="G3">
+        <v>211</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B4">
-        <v>30.22</v>
+        <v>8.4</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D4">
-        <v>38.619999999999997</v>
+        <v>6.24</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>246</v>
+        <v>34</v>
       </c>
       <c r="G4">
-        <v>190</v>
+        <v>251</v>
       </c>
       <c r="H4">
-        <v>61</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5">
-        <v>28.22</v>
+        <v>65.53</v>
       </c>
       <c r="C5">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>9.82</v>
+        <v>132.02000000000001</v>
       </c>
       <c r="E5">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>68</v>
+        <v>953</v>
       </c>
       <c r="G5">
-        <v>211</v>
+        <v>185</v>
       </c>
       <c r="H5">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6">
-        <v>8.4</v>
+        <v>7.16</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6">
-        <v>6.24</v>
+        <v>2.35</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G6">
         <v>251</v>
@@ -1539,48 +1647,48 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B7">
-        <v>65.53</v>
+        <v>7.3</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>132.02000000000001</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>953</v>
+        <v>14</v>
       </c>
       <c r="G7">
-        <v>185</v>
+        <v>251</v>
       </c>
       <c r="H7">
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8">
-        <v>7.16</v>
+        <v>2.13</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>2.35</v>
+        <v>2.15</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G8">
         <v>251</v>
@@ -1589,101 +1697,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9">
-        <v>7.3</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="E9">
+    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.62</v>
+      </c>
+      <c r="C9" s="5">
         <v>1</v>
       </c>
-      <c r="F9">
-        <v>14</v>
-      </c>
-      <c r="G9">
+      <c r="D9" s="5">
+        <v>1.05</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5">
         <v>251</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10">
-        <v>2.13</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>2.15</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>28</v>
-      </c>
-      <c r="G10">
-        <v>251</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1.62</v>
-      </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1.05</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>6</v>
-      </c>
-      <c r="G11" s="5">
-        <v>251</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
+    <row r="11" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1691,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF30A77-3566-8C4B-92CC-3F903D073C1A}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1708,152 +1764,177 @@
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>59</v>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2">
+        <v>1.62</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1.06</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3">
-        <v>1.62</v>
+        <v>2.13</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>1.06</v>
+        <v>2.15</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="H3">
-        <v>190</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4">
-        <v>2.13</v>
+        <v>1.64</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>2.15</v>
+        <v>1.07</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="H4">
-        <v>211</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C5">
-        <v>1.64</v>
+        <v>2.14</v>
       </c>
       <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2.16</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>1.07</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="G5">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="H5">
-        <v>251</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C6">
-        <v>2.14</v>
+        <v>1.62</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>2.16</v>
+        <v>1.06</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="H6">
-        <v>185</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C7">
-        <v>1.62</v>
+        <v>1.65</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1.06</v>
+        <v>1.08</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1867,97 +1948,71 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C8">
-        <v>1.65</v>
+        <v>2.13</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>1.08</v>
+        <v>2.15</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="H8">
         <v>251</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9">
-        <v>2.13</v>
-      </c>
-      <c r="D9">
+    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2.15</v>
+      </c>
+      <c r="D9" s="5">
         <v>2</v>
       </c>
-      <c r="E9">
-        <v>2.15</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="5">
+        <v>2.16</v>
+      </c>
+      <c r="F9" s="5">
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="5">
         <v>28</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <v>251</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="5">
-        <v>2.15</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5">
-        <v>2.16</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5">
-        <v>28</v>
-      </c>
-      <c r="H10" s="5">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
+    <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1967,8 +2022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2AB93A-F0D0-0E4F-9A89-9C7CA62FFC75}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1979,153 +2034,153 @@
   <sheetData>
     <row r="1" spans="1:6" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:6" s="27" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="D2" s="26">
+        <v>2514</v>
+      </c>
+      <c r="E2" s="26">
+        <v>26</v>
+      </c>
+      <c r="F2" s="27">
+        <v>256003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="27" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="C3" s="28" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="33" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="D3" s="26">
+        <v>105</v>
+      </c>
+      <c r="E3" s="26">
+        <v>102</v>
+      </c>
+      <c r="F3" s="27">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="27" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="26">
+        <v>960</v>
+      </c>
+      <c r="E4" s="26">
+        <v>596</v>
+      </c>
+      <c r="F4" s="27">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="27" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="27">
-        <v>2514</v>
-      </c>
-      <c r="E2" s="27">
-        <v>26</v>
-      </c>
-      <c r="F2" s="33">
-        <v>256003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="33" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="34" t="s">
+      <c r="B5" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="27">
-        <v>105</v>
-      </c>
-      <c r="E3" s="27">
-        <v>102</v>
-      </c>
-      <c r="F3" s="33">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="33" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="C5" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="D5" s="26">
+        <v>778</v>
+      </c>
+      <c r="E5" s="26">
+        <v>19</v>
+      </c>
+      <c r="F5" s="27">
+        <v>181555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="27" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="B6" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="27">
-        <v>960</v>
-      </c>
-      <c r="E4" s="27">
-        <v>596</v>
-      </c>
-      <c r="F4" s="33">
-        <v>1995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="33" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="34" t="s">
+      <c r="C6" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="D6" s="26">
+        <v>31</v>
+      </c>
+      <c r="E6" s="26">
+        <v>17</v>
+      </c>
+      <c r="F6" s="27">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="27" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="27">
-        <v>778</v>
-      </c>
-      <c r="E5" s="27">
-        <v>19</v>
-      </c>
-      <c r="F5" s="33">
-        <v>181555</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="33" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="B7" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="C7" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="27">
-        <v>31</v>
-      </c>
-      <c r="E6" s="27">
-        <v>17</v>
-      </c>
-      <c r="F6" s="33">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="33" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="36" t="s">
+      <c r="D7" s="31">
+        <v>63</v>
+      </c>
+      <c r="E7" s="31">
+        <v>14</v>
+      </c>
+      <c r="F7" s="29">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="226" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="37">
-        <v>63</v>
-      </c>
-      <c r="E7" s="37">
-        <v>14</v>
-      </c>
-      <c r="F7" s="35">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add read depths to Table S1
</commit_message>
<xml_diff>
--- a/supp_tables.xlsx
+++ b/supp_tables.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wickr/Library/CloudStorage/Dropbox/Uni_research/Projects/2024-01_low-depth_polishing_paper/depth_vs_polishing_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E755977-9EBA-5647-9600-05C8931AD965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3842647D-723C-A147-9D0C-59FF7C554804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
+    <workbookView xWindow="1100" yWindow="-25980" windowWidth="30240" windowHeight="17180" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table S1, accessions" sheetId="2" r:id="rId1"/>
+    <sheet name="Table S1, reads and accessions" sheetId="2" r:id="rId1"/>
     <sheet name="Table S2, Medaka polishing" sheetId="1" r:id="rId2"/>
     <sheet name="Table S3, Single &gt;25x" sheetId="5" r:id="rId3"/>
     <sheet name="Table S4, Combination &gt;25x" sheetId="4" r:id="rId4"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="190">
   <si>
     <t>Genome</t>
   </si>
@@ -1634,6 +1634,12 @@
       <t>: Medaka-polishing results. 
 Of the nine ONT-only assemblies used in this study, three improved (blue) with Medaka v1.11.3 polishing (r1041_e82_400bps_sup_v4.3.0 model), three did not change, three got worse (red), and Medaka made the total error count worse. We therefore do not recommend using Medaka to polish Trycycler assemblies of sup-basecalled ONT reads.</t>
     </r>
+  </si>
+  <si>
+    <t>ONT read depth</t>
+  </si>
+  <si>
+    <t>Illumina read depth</t>
   </si>
 </sst>
 </file>
@@ -1751,7 +1757,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1768,20 +1774,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1810,13 +1807,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1837,12 +1827,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1885,6 +1869,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2205,9 +2195,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329A5B2C-B2CD-2E4C-9B25-8D30DFCCCE6A}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2217,24 +2209,30 @@
     <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -2250,8 +2248,14 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>1982.4</v>
+      </c>
+      <c r="G2">
+        <v>472.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -2267,8 +2271,14 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>1807.1</v>
+      </c>
+      <c r="G3">
+        <v>272.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -2284,8 +2294,14 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>1805.6</v>
+      </c>
+      <c r="G4">
+        <v>106.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -2301,8 +2317,14 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>1562.8</v>
+      </c>
+      <c r="G5">
+        <v>315.89999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>173</v>
       </c>
@@ -2318,8 +2340,14 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>1709.8</v>
+      </c>
+      <c r="G6">
+        <v>307.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>174</v>
       </c>
@@ -2335,8 +2363,14 @@
       <c r="E7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>2353.4</v>
+      </c>
+      <c r="G7">
+        <v>54.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>175</v>
       </c>
@@ -2352,8 +2386,14 @@
       <c r="E8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>3051.4</v>
+      </c>
+      <c r="G8">
+        <v>380.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>176</v>
       </c>
@@ -2369,8 +2409,14 @@
       <c r="E9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>657.2</v>
+      </c>
+      <c r="G9">
+        <v>137.30000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>177</v>
       </c>
@@ -2386,19 +2432,27 @@
       <c r="E10" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
+      <c r="F10" s="5">
+        <v>1181.8</v>
+      </c>
+      <c r="G10" s="5">
+        <v>527.70000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2409,7 +2463,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:F14"/>
+      <selection activeCell="B3" sqref="B3:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2423,14 +2477,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="37"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2466,10 +2520,10 @@
         <f>CONCATENATE("Q", IF(C3=0, "∞", ROUND(-10*LOG10(C3/$B3), 1)))</f>
         <v>Q55.5</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="18">
         <v>3</v>
       </c>
-      <c r="F3" s="22" t="str">
+      <c r="F3" s="19" t="str">
         <f>CONCATENATE("Q", IF(E3=0, "∞", ROUND(-10*LOG10(E3/$B3), 1)))</f>
         <v>Q57.7</v>
       </c>
@@ -2488,10 +2542,10 @@
         <f t="shared" ref="D4:F12" si="0">CONCATENATE("Q", IF(C4=0, "∞", ROUND(-10*LOG10(C4/$B4), 1)))</f>
         <v>Q49.2</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="14">
         <v>28</v>
       </c>
-      <c r="F4" s="18" t="str">
+      <c r="F4" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Q47.3</v>
       </c>
@@ -2532,10 +2586,10 @@
         <f t="shared" si="0"/>
         <v>Q57.7</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="18">
         <v>4</v>
       </c>
-      <c r="F6" s="22" t="str">
+      <c r="F6" s="19" t="str">
         <f t="shared" si="0"/>
         <v>Q58.6</v>
       </c>
@@ -2598,10 +2652,10 @@
         <f t="shared" si="0"/>
         <v>Q62</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="14">
         <v>6</v>
       </c>
-      <c r="F9" s="18" t="str">
+      <c r="F9" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Q59</v>
       </c>
@@ -2620,10 +2674,10 @@
         <f t="shared" si="0"/>
         <v>Q63.2</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>3</v>
       </c>
-      <c r="F10" s="18" t="str">
+      <c r="F10" s="15" t="str">
         <f t="shared" si="0"/>
         <v>Q61.4</v>
       </c>
@@ -2632,20 +2686,20 @@
       <c r="A11" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="6">
         <v>5147091</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="7">
         <v>2</v>
       </c>
-      <c r="D11" s="14" t="str">
+      <c r="D11" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Q64.1</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="35">
         <v>1</v>
       </c>
-      <c r="F11" s="24" t="str">
+      <c r="F11" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Q67.1</v>
       </c>
@@ -2666,24 +2720,24 @@
         <f t="shared" si="0"/>
         <v>Q59.3</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="16">
         <f>SUM(E3:E11)</f>
         <v>47</v>
       </c>
-      <c r="F12" s="20" t="str">
+      <c r="F12" s="17" t="str">
         <f t="shared" si="0"/>
         <v>Q58.2</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="110" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2719,28 +2773,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2953,18 +3007,18 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2994,28 +3048,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="12" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3228,16 +3282,16 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3262,154 +3316,154 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="26" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:6" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="20">
         <v>2514</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="20">
         <v>26</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="21">
         <v>256003</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="26" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+    <row r="3" spans="1:6" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="20">
         <v>105</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="20">
         <v>102</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="21">
         <v>899</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="26" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:6" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="20">
         <v>960</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="20">
         <v>596</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="21">
         <v>1995</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="26" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:6" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="20">
         <v>778</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="20">
         <v>19</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="21">
         <v>181555</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="26" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:6" s="21" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="20">
         <v>31</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="20">
         <v>17</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="21">
         <v>587</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="26" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+    <row r="7" spans="1:6" s="21" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="25">
         <v>63</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="25">
         <v>14</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="23">
         <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="226" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3442,876 +3496,876 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="41" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="27" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="28">
         <v>1</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="28">
         <v>1</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
     </row>
     <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="28">
         <v>1</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
     </row>
     <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
     </row>
     <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="28">
         <v>1</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
     </row>
     <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="28">
         <v>1</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
     </row>
     <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="28">
         <v>1</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
     </row>
     <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="28">
         <v>1</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
     </row>
     <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="28">
         <v>1</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="G10" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
     </row>
     <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="29">
         <v>3</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="G11" s="33" t="s">
+      <c r="G11" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
     </row>
     <row r="12" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="28">
         <v>1</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
     </row>
     <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="29">
         <v>2</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
     </row>
     <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33" t="s">
+      <c r="D14" s="28"/>
+      <c r="E14" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
     </row>
     <row r="15" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33" t="s">
+      <c r="D15" s="28"/>
+      <c r="E15" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
     </row>
     <row r="16" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33" t="s">
+      <c r="D16" s="28"/>
+      <c r="E16" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33" t="s">
+      <c r="D17" s="28"/>
+      <c r="E17" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33" t="s">
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="J17" s="33" t="s">
+      <c r="J17" s="28" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33" t="s">
+      <c r="D18" s="28"/>
+      <c r="E18" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33" t="s">
+      <c r="G18" s="28"/>
+      <c r="H18" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="I18" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="J18" s="28" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33" t="s">
+      <c r="D19" s="28"/>
+      <c r="E19" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33" t="s">
+      <c r="G19" s="28"/>
+      <c r="H19" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="J19" s="33" t="s">
+      <c r="J19" s="28" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="28">
         <v>1</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33" t="s">
+      <c r="H20" s="28"/>
+      <c r="I20" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="J20" s="33"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="21" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33" t="s">
+      <c r="D21" s="28"/>
+      <c r="E21" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33" t="s">
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="J21" s="33" t="s">
+      <c r="J21" s="28" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33" t="s">
+      <c r="D22" s="28"/>
+      <c r="E22" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33" t="s">
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="J22" s="33" t="s">
+      <c r="J22" s="28" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="29">
         <v>3</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33" t="s">
+      <c r="H23" s="28"/>
+      <c r="I23" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="J23" s="33"/>
+      <c r="J23" s="28"/>
     </row>
     <row r="24" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33" t="s">
+      <c r="D24" s="28"/>
+      <c r="E24" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33" t="s">
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="J24" s="33"/>
+      <c r="J24" s="28"/>
     </row>
     <row r="25" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33" t="s">
+      <c r="D25" s="28"/>
+      <c r="E25" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33" t="s">
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="J25" s="33" t="s">
+      <c r="J25" s="28" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33" t="s">
+      <c r="D26" s="28"/>
+      <c r="E26" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F26" s="33" t="s">
+      <c r="F26" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33" t="s">
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="J26" s="33" t="s">
+      <c r="J26" s="28" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33" t="s">
+      <c r="D27" s="28"/>
+      <c r="E27" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33" t="s">
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="J27" s="33" t="s">
+      <c r="J27" s="28" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33" t="s">
+      <c r="D28" s="28"/>
+      <c r="E28" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F28" s="33" t="s">
+      <c r="F28" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33" t="s">
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="J28" s="33" t="s">
+      <c r="J28" s="28" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33" t="s">
+      <c r="D29" s="28"/>
+      <c r="E29" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F29" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33" t="s">
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="J29" s="33" t="s">
+      <c r="J29" s="28" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33" t="s">
+      <c r="D30" s="28"/>
+      <c r="E30" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F30" s="33" t="s">
+      <c r="F30" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33" t="s">
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="J30" s="33" t="s">
+      <c r="J30" s="28" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="D31" s="33">
+      <c r="D31" s="28">
         <v>1</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33" t="s">
+      <c r="G31" s="28"/>
+      <c r="H31" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="I31" s="33" t="s">
+      <c r="I31" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="J31" s="33" t="s">
+      <c r="J31" s="28" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33" t="s">
+      <c r="D32" s="28"/>
+      <c r="E32" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F32" s="33" t="s">
+      <c r="F32" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33" t="s">
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="J32" s="33" t="s">
+      <c r="J32" s="28" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="35">
+      <c r="D33" s="30">
         <v>1</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="F33" s="35" t="s">
+      <c r="F33" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="G33" s="35" t="s">
+      <c r="G33" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="32"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="27"/>
     </row>
     <row r="36" spans="1:10" ht="157" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Change supp table order
</commit_message>
<xml_diff>
--- a/supp_tables.xlsx
+++ b/supp_tables.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wickr/Library/CloudStorage/Dropbox/Uni_research/Projects/2024-01_low-depth_polishing_paper/depth_vs_polishing_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3842647D-723C-A147-9D0C-59FF7C554804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ED810B-FD1F-9047-BAA6-6F36126880FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="-25980" windowWidth="30240" windowHeight="17180" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
+    <workbookView xWindow="1100" yWindow="-25980" windowWidth="32120" windowHeight="21500" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1, reads and accessions" sheetId="2" r:id="rId1"/>
-    <sheet name="Table S2, Medaka polishing" sheetId="1" r:id="rId2"/>
-    <sheet name="Table S3, Single &gt;25x" sheetId="5" r:id="rId3"/>
-    <sheet name="Table S4, Combination &gt;25x" sheetId="4" r:id="rId4"/>
-    <sheet name="Table S5, Param optimisation" sheetId="6" r:id="rId5"/>
-    <sheet name="Table S6, Error Characterisatio" sheetId="8" r:id="rId6"/>
+    <sheet name="Table S2, ONT assembly errors" sheetId="8" r:id="rId2"/>
+    <sheet name="Table S3, Medaka polishing" sheetId="1" r:id="rId3"/>
+    <sheet name="Table S4, Single &gt;25x" sheetId="5" r:id="rId4"/>
+    <sheet name="Table S5, Combination &gt;25x" sheetId="4" r:id="rId5"/>
+    <sheet name="Table S6, Param optimisation" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="188">
   <si>
     <t>Genome</t>
   </si>
@@ -417,9 +417,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Indel Size (bp)</t>
-  </si>
-  <si>
     <t>Base</t>
   </si>
   <si>
@@ -438,27 +435,15 @@
     <t>C</t>
   </si>
   <si>
-    <t>6-&gt;5</t>
-  </si>
-  <si>
     <t>chromosome 2716540-2716570</t>
   </si>
   <si>
     <t>T</t>
   </si>
   <si>
-    <t>10-&gt;9</t>
-  </si>
-  <si>
     <t>plasmid 12153-12183</t>
   </si>
   <si>
-    <t>22-&gt;21</t>
-  </si>
-  <si>
-    <t>See Supplementary Figure 1</t>
-  </si>
-  <si>
     <t>chromosome_1 1469614-1469644</t>
   </si>
   <si>
@@ -468,18 +453,12 @@
     <t>N</t>
   </si>
   <si>
-    <t>C-&gt;T</t>
-  </si>
-  <si>
     <t>chromosome_1 1475138-1475168</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>9-&gt;8</t>
-  </si>
-  <si>
     <t>chromosome_1 970393-970423</t>
   </si>
   <si>
@@ -489,42 +468,24 @@
     <t>chromosome 808078-808108</t>
   </si>
   <si>
-    <t>12-&gt;11</t>
-  </si>
-  <si>
     <t>chromosome 1127972-1128002</t>
   </si>
   <si>
-    <t>11-&gt;10</t>
-  </si>
-  <si>
     <t>chromosome 2671888-2671920</t>
   </si>
   <si>
-    <t>24-&gt;21</t>
-  </si>
-  <si>
     <t>chromosome 864434-864464</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
-    <t>8-&gt;7</t>
-  </si>
-  <si>
     <t>chromosome 148683-148714</t>
   </si>
   <si>
-    <t>13-&gt;11</t>
-  </si>
-  <si>
     <t>chromosome 1493758-1493788</t>
   </si>
   <si>
-    <t>G-&gt;A</t>
-  </si>
-  <si>
     <t>chromosome 1576238-1576268</t>
   </si>
   <si>
@@ -552,9 +513,6 @@
     <t>chromosome 548170-548202</t>
   </si>
   <si>
-    <t>22-&gt;19</t>
-  </si>
-  <si>
     <t>chromosome 568539-568569</t>
   </si>
   <si>
@@ -582,49 +540,599 @@
     <t>Insertion</t>
   </si>
   <si>
-    <t>T-&gt;TT</t>
-  </si>
-  <si>
     <t>chromosome 1359690-1359720</t>
   </si>
   <si>
     <t>chromosome 918458-918488</t>
   </si>
   <si>
-    <t>Error Region (contig and coordinates)</t>
-  </si>
-  <si>
-    <t>Homopolymer (Y = Yes, N = No)</t>
-  </si>
-  <si>
-    <t>Error Region with Methylation (6mA Methylation in Blue, Error in Red)</t>
-  </si>
-  <si>
-    <t>Methylated Base(s)</t>
-  </si>
-  <si>
-    <t>AT</t>
-  </si>
-  <si>
-    <t>Deletion Homopolymer Size Change</t>
-  </si>
-  <si>
     <t>No 6mA methylation in the region</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Campylobacter jejuni</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-33560)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Campylobacter lari</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-35221)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Escherichia coli</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-25922)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Listeria ivanovii</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-19119)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Listeria monocytogenes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-BAA-679)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Listeria welshimeri </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ATCC-35897)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Salmonella enterica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-10708)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vibrio cholerae</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-14035)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vibrio parahaemolyticus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-17802)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Table S2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Medaka-polishing results. 
+Of the nine ONT-only assemblies used in this study, three improved (blue) with Medaka v1.11.3 polishing (r1041_e82_400bps_sup_v4.3.0 model), three did not change, three got worse (red), and Medaka made the total error count worse. We therefore do not recommend using Medaka to polish Trycycler assemblies of sup-basecalled ONT reads.</t>
+    </r>
+  </si>
+  <si>
+    <t>ONT read depth</t>
+  </si>
+  <si>
+    <t>Illumina read depth</t>
+  </si>
+  <si>
+    <t>See Figure S1</t>
+  </si>
+  <si>
+    <t>6→5</t>
+  </si>
+  <si>
+    <t>10→9</t>
+  </si>
+  <si>
+    <t>22→21</t>
+  </si>
+  <si>
+    <t>9→8</t>
+  </si>
+  <si>
+    <t>12→11</t>
+  </si>
+  <si>
+    <t>11→10</t>
+  </si>
+  <si>
+    <t>24→21</t>
+  </si>
+  <si>
+    <t>8→7</t>
+  </si>
+  <si>
+    <t>13→11</t>
+  </si>
+  <si>
+    <t>22→19</t>
+  </si>
+  <si>
+    <t>T→TT</t>
+  </si>
+  <si>
+    <t>C→T</t>
+  </si>
+  <si>
+    <t>G→A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Table S6: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Detailed error characterisation for each error between the long-read only Trycycler genomes (the ones that were polished) and the reference genome. One error is characterised in detail in the manuscript (Supplementary Figure 1): the extra-long homopolymer on the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Salmonella enterica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (ATCC-10708) plasmid, row 4. All deletions between reference and the long-read only assemblies occured in homolopolymers. Three regions have multiple errors i.e. where the deletion observed was larger than size 1 (rows 11, 13 and 23). For </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Campylobacter lari</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (ATCC-35221), 13/16 errors observed were SNP errors. Therefore, we decided to conduct a methylation analysis of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>C. lari</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> with MicrobeMod (github.com/cultivarium/MicrobeMod) to determine if there were methylated bases near the SNPs. Column I shows the error region of each </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Campylobacter lari</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> error with incorrect bases coloured red and methylated bases coloured blue</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> There was at least one 6mA methylated base near every SNP except 1 (row 24), with most occuring within 2 bases. </t>
+    </r>
+  </si>
+  <si>
+    <t>Error region (contig and coordinates)</t>
+  </si>
+  <si>
+    <t>Indel size (bp)</t>
+  </si>
+  <si>
+    <t>Homopolymer</t>
+  </si>
+  <si>
+    <t>Homopolymer size change</t>
+  </si>
+  <si>
+    <t>Error region with methylation (6mA methylation in blue, error in eed)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Salmonella enterica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-10708)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vibrio cholerae</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-14035)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vibrio parahaemolyticus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ATCC-17802)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Listeria ivanovii </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ATCC-19119)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Escherichia coli </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ATCC-25922)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Campylobacter jejuni</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (ATCC-33560)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Campylobacter lari </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ATCC-35221)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>TCAAACCTTTG</t>
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
       <t>A</t>
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -632,7 +1140,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -640,7 +1148,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -655,7 +1163,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -664,14 +1172,14 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
       <t>A</t>
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -679,7 +1187,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -689,7 +1197,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -697,14 +1205,14 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
       <t>ATC</t>
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -713,7 +1221,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -725,7 +1233,7 @@
   <si>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -734,14 +1242,14 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
       <t>AT</t>
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -750,14 +1258,14 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
       <t>GA</t>
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -765,7 +1273,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -773,7 +1281,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -788,7 +1296,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -796,7 +1304,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -804,7 +1312,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -819,7 +1327,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -827,7 +1335,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -837,7 +1345,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -845,7 +1353,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -860,7 +1368,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -868,7 +1376,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -876,7 +1384,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -891,7 +1399,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -899,7 +1407,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -909,7 +1417,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -917,7 +1425,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -932,7 +1440,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -940,7 +1448,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -948,7 +1456,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -963,7 +1471,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -971,7 +1479,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -979,7 +1487,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -994,7 +1502,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -1002,7 +1510,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1012,7 +1520,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -1020,7 +1528,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1035,7 +1543,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -1043,7 +1551,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -1051,7 +1559,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1066,7 +1574,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -1074,7 +1582,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1084,7 +1592,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -1092,7 +1600,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1107,7 +1615,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -1115,7 +1623,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1125,7 +1633,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color rgb="FF00B0F0"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
@@ -1133,7 +1641,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1152,121 +1660,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Campylobacter jejuni</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-33560)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Campylobacter lari</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-35221)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Escherichia coli</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-25922)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Listeria ivanovii</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-19119)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Listeria monocytogenes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-BAA-679)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Listeria welshimeri </t>
     </r>
     <r>
@@ -1279,367 +1672,6 @@
       </rPr>
       <t>(ATCC-35897)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Salmonella enterica</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-10708)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vibrio cholerae</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-14035)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vibrio parahaemolyticus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-17802)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Salmonella enterica</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-10708)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vibrio cholerae</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-14035)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vibrio parahaemolyticus </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(ATCC-17802)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Listeria ivanovii </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(ATCC-19119)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Escherichia coli </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(ATCC-25922)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Campylobacter jejuni</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> (ATCC-33560)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Campylobacter lari </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(ATCC-35221)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Listeria welshimeri </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(ATCC-35897)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Table S6: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Detailed error characterisation for each error between the long-read only Trycycler genomes (the ones that were polished) and the reference genome. One error is characterised in detail in the manuscript (Supplementary Figure 1): the extra-long homopolymer on the </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Salmonella enterica</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (ATCC-10708) plasmid, row 4. All deletions between reference and the long-read only assemblies occured in homolopolymers. Three regions have multiple errors i.e. where the deletion observed was larger than size 1 (rows 11, 13 and 23). For </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Campylobacter lari</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t> (ATCC-35221), 13/16 errors observed were SNP errors. Therefore, we decided to conduct a methylation analysis of _C. lari_ with MicrobeMod (https://github.com/cultivarium/MicrobeMod) to determine if there were methylated bases near the SNPs. Column I shows the error region of each Campylobacter lari</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> error with incorrect bases coloured red and methylated bases coloured blue.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> There was at least one 6mA methylated base near every SNP except 1 (row 24), with most occuring within 2 bases. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Table S2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: Medaka-polishing results. 
-Of the nine ONT-only assemblies used in this study, three improved (blue) with Medaka v1.11.3 polishing (r1041_e82_400bps_sup_v4.3.0 model), three did not change, three got worse (red), and Medaka made the total error count worse. We therefore do not recommend using Medaka to polish Trycycler assemblies of sup-basecalled ONT reads.</t>
-    </r>
-  </si>
-  <si>
-    <t>ONT read depth</t>
-  </si>
-  <si>
-    <t>Illumina read depth</t>
   </si>
 </sst>
 </file>
@@ -1649,7 +1681,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1694,44 +1726,28 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
+      <sz val="12"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FF00B0F0"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
     <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="14"/>
-      <color theme="1"/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1778,7 +1794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1850,14 +1866,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1875,6 +1883,11 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2197,9 +2210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329A5B2C-B2CD-2E4C-9B25-8D30DFCCCE6A}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2226,15 +2237,15 @@
         <v>7</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>188</v>
+        <v>145</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -2257,7 +2268,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -2280,7 +2291,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -2303,7 +2314,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -2326,7 +2337,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -2349,7 +2360,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
@@ -2372,7 +2383,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
@@ -2395,7 +2406,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
         <v>34</v>
@@ -2418,7 +2429,7 @@
     </row>
     <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>35</v>
@@ -2440,15 +2451,15 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2459,6 +2470,847 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1F38ED-336F-E241-A27A-3D55AF4798CF}">
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.5" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="40.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="33">
+        <v>1</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="33">
+        <v>1</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="33">
+        <v>1</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="I4" s="33"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="33">
+        <v>1</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="33">
+        <v>1</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="33">
+        <v>1</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="33">
+        <v>1</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="34">
+        <v>3</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="33">
+        <v>1</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="34">
+        <v>2</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="33">
+        <v>1</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="34">
+        <v>3</v>
+      </c>
+      <c r="E23" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="33">
+        <v>1</v>
+      </c>
+      <c r="E31" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="35">
+        <v>1</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+    </row>
+    <row r="35" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A35:I35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CD79FE-3416-9E47-B0D5-3F9B64FD8358}">
   <dimension ref="A1:F14"/>
   <sheetViews>
@@ -2477,14 +3329,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="32"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -2508,7 +3360,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="B3" s="3">
         <v>1768448</v>
@@ -2530,7 +3382,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="B4" s="3">
         <v>1513368</v>
@@ -2552,7 +3404,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="B5" s="3">
         <v>5204893</v>
@@ -2574,7 +3426,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B6" s="3">
         <v>2919549</v>
@@ -2596,7 +3448,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B7" s="3">
         <v>2944530</v>
@@ -2618,7 +3470,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B8" s="3">
         <v>2814137</v>
@@ -2640,7 +3492,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B9" s="3">
         <v>4801704</v>
@@ -2662,7 +3514,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B10" s="3">
         <v>4142374</v>
@@ -2684,7 +3536,7 @@
     </row>
     <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B11" s="6">
         <v>5147091</v>
@@ -2696,10 +3548,10 @@
         <f t="shared" si="0"/>
         <v>Q64.1</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="31">
         <v>1</v>
       </c>
-      <c r="F11" s="36" t="str">
+      <c r="F11" s="32" t="str">
         <f t="shared" si="0"/>
         <v>Q67.1</v>
       </c>
@@ -2730,14 +3582,14 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="110" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
+      <c r="A14" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2752,12 +3604,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2A52BF-89B5-F84A-9572-1BEA1D441973}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:H11"/>
+      <selection activeCell="H25" sqref="H25:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3007,16 +3859,16 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
     </row>
@@ -3028,7 +3880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF30A77-3566-8C4B-92CC-3F903D073C1A}">
   <dimension ref="A1:H11"/>
   <sheetViews>
@@ -3282,16 +4134,16 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3301,7 +4153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2AB93A-F0D0-0E4F-9A89-9C7CA62FFC75}">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -3456,14 +4308,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="226" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3471,906 +4323,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1F38ED-336F-E241-A27A-3D55AF4798CF}">
-  <dimension ref="A1:J36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="41" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="28">
-        <v>1</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-    </row>
-    <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="28">
-        <v>1</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-    </row>
-    <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="28">
-        <v>1</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-    </row>
-    <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-    </row>
-    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="28">
-        <v>1</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-    </row>
-    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="28">
-        <v>1</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-    </row>
-    <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="28">
-        <v>1</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-    </row>
-    <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D9" s="28">
-        <v>1</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-    </row>
-    <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="28">
-        <v>1</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-    </row>
-    <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="29">
-        <v>3</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-    </row>
-    <row r="12" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="28">
-        <v>1</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-    </row>
-    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="29">
-        <v>2</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-    </row>
-    <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-    </row>
-    <row r="15" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-    </row>
-    <row r="16" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-    </row>
-    <row r="17" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="J17" s="28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="J18" s="28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="I19" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="J19" s="28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="28">
-        <v>1</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="J20" s="28"/>
-    </row>
-    <row r="21" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="J21" s="28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="J22" s="28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="29">
-        <v>3</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="J23" s="28"/>
-    </row>
-    <row r="24" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F24" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="J24" s="28"/>
-    </row>
-    <row r="25" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="J25" s="28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F26" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="J26" s="28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="J27" s="28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F28" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="J28" s="28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F29" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="J29" s="28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="J30" s="28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="D31" s="28">
-        <v>1</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="I31" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="J31" s="28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F32" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="J32" s="28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="30">
-        <v>1</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="G33" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="27"/>
-    </row>
-    <row r="36" spans="1:10" ht="157" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A36:H36"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
consistent capitalisation and order plus trim captions Fig S1 S4
</commit_message>
<xml_diff>
--- a/supp_tables.xlsx
+++ b/supp_tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wickr/Library/CloudStorage/Dropbox/Uni_research/Projects/2024-01_low-depth_polishing_paper/depth_vs_polishing_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1667917/Documents/Wick/depth_vs_polishing_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16ED810B-FD1F-9047-BAA6-6F36126880FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AFAC30-1E45-2545-A3B1-F5CA801409AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="-25980" windowWidth="32120" windowHeight="21500" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" activeTab="1" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1, reads and accessions" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="189">
   <si>
     <t>Genome</t>
   </si>
@@ -828,122 +828,6 @@
     <t>G→A</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Table S6: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Detailed error characterisation for each error between the long-read only Trycycler genomes (the ones that were polished) and the reference genome. One error is characterised in detail in the manuscript (Supplementary Figure 1): the extra-long homopolymer on the </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Salmonella enterica</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (ATCC-10708) plasmid, row 4. All deletions between reference and the long-read only assemblies occured in homolopolymers. Three regions have multiple errors i.e. where the deletion observed was larger than size 1 (rows 11, 13 and 23). For </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Campylobacter lari</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (ATCC-35221), 13/16 errors observed were SNP errors. Therefore, we decided to conduct a methylation analysis of </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>C. lari</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> with MicrobeMod (github.com/cultivarium/MicrobeMod) to determine if there were methylated bases near the SNPs. Column I shows the error region of each </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Campylobacter lari</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> error with incorrect bases coloured red and methylated bases coloured blue</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> There was at least one 6mA methylated base near every SNP except 1 (row 24), with most occuring within 2 bases. </t>
-    </r>
-  </si>
-  <si>
     <t>Error region (contig and coordinates)</t>
   </si>
   <si>
@@ -1671,6 +1555,125 @@
         <scheme val="minor"/>
       </rPr>
       <t>(ATCC-35897)</t>
+    </r>
+  </si>
+  <si>
+    <t>Substitution</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Table S6: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Detailed error characterisation for each error between the long-read only Trycycler genomes (the ones that were polished) and the reference genome. One error is characterised in detail in the manuscript (Supplementary Figure 1): the extra-long homopolymer on the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Salmonella enterica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (ATCC-10708) plasmid, row 4. All deletions between reference and the long-read only assemblies occured in homolopolymers. Three regions have multiple errors i.e. where the deletion observed was larger than size 1 (rows 11, 13 and 23). For </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Campylobacter lari</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (ATCC-35221), 13/16 errors observed were substitution errors. Therefore, we decided to conduct a methylation analysis of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>C. lari</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> with MicrobeMod (github.com/cultivarium/MicrobeMod) to determine if there were methylated bases near the substitutionss. Column I shows the error region of each </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Campylobacter lari</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> error with incorrect bases coloured red and methylated bases coloured blue</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> There was at least one 6mA methylated base near every substitution except one (row 24), with most occuring within 2 bases. </t>
     </r>
   </si>
 </sst>
@@ -1681,7 +1684,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1724,13 +1727,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1794,7 +1790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1866,7 +1862,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1875,17 +1884,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2210,7 +2209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329A5B2C-B2CD-2E4C-9B25-8D30DFCCCE6A}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2451,15 +2450,15 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2473,15 +2472,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1F38ED-336F-E241-A27A-3D55AF4798CF}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="6" max="6" width="7.5" customWidth="1"/>
@@ -2495,812 +2494,735 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>90</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>163</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>164</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>91</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H1" s="13" t="s">
         <v>92</v>
       </c>
       <c r="I1" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="33" t="s">
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E6" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="33" t="s">
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E7" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="29">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" t="s">
+        <v>111</v>
+      </c>
+      <c r="G12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="29">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>171</v>
+      </c>
+      <c r="B14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" t="s">
+        <v>159</v>
+      </c>
+      <c r="I17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H18" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" t="s">
+        <v>159</v>
+      </c>
+      <c r="H19" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" t="s">
         <v>149</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="33" t="s">
+      <c r="I20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" t="s">
+        <v>102</v>
+      </c>
+      <c r="I22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D23" s="29">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" t="s">
+        <v>157</v>
+      </c>
+      <c r="I23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" t="s">
+        <v>160</v>
+      </c>
+      <c r="I24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>172</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" t="s">
+        <v>159</v>
+      </c>
+      <c r="I26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>172</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E27" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" t="s">
+        <v>159</v>
+      </c>
+      <c r="I27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>172</v>
+      </c>
+      <c r="B28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" t="s">
+        <v>159</v>
+      </c>
+      <c r="I28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" t="s">
+        <v>160</v>
+      </c>
+      <c r="I29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" t="s">
+        <v>159</v>
+      </c>
+      <c r="I30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31">
         <v>1</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E31" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" t="s">
+        <v>98</v>
+      </c>
+      <c r="H31" t="s">
+        <v>158</v>
+      </c>
+      <c r="I31" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>172</v>
+      </c>
+      <c r="B32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" t="s">
+        <v>159</v>
+      </c>
+      <c r="I32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="30">
+        <v>1</v>
+      </c>
+      <c r="E33" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="H4" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="I4" s="33"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="33">
-        <v>1</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="G6" s="33" t="s">
+      <c r="F33" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="33">
-        <v>1</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D8" s="33">
-        <v>1</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="33">
-        <v>1</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="33">
-        <v>1</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="34">
-        <v>3</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="33">
-        <v>1</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="34">
-        <v>2</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="I18" s="33" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="I19" s="33" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="33">
-        <v>1</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G20" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>120</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F21" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="34">
-        <v>3</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G23" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F27" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B28" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F30" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="D31" s="33">
-        <v>1</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="I31" s="33" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F32" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="B33" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="C33" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" s="35">
-        <v>1</v>
-      </c>
-      <c r="E33" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="F33" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="G33" s="35" t="s">
-        <v>151</v>
-      </c>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
     </row>
     <row r="35" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
+      <c r="A35" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3329,14 +3251,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="28"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -3548,10 +3470,10 @@
         <f t="shared" si="0"/>
         <v>Q64.1</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="27">
         <v>1</v>
       </c>
-      <c r="F11" s="32" t="str">
+      <c r="F11" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Q67.1</v>
       </c>
@@ -3582,14 +3504,14 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="110" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3859,16 +3781,16 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
     </row>
@@ -4134,16 +4056,16 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4308,14 +4230,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="226" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
minor changes to supp figure numbers
</commit_message>
<xml_diff>
--- a/supp_tables.xlsx
+++ b/supp_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1667917/Documents/Wick/depth_vs_polishing_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AFAC30-1E45-2545-A3B1-F5CA801409AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BF9E88-1235-AC4F-8FFB-D6C796527BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" activeTab="1" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" xr2:uid="{E0E4A5C3-8AA8-C14D-BB15-E5B845EF2FCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1, reads and accessions" sheetId="2" r:id="rId1"/>
@@ -1790,7 +1790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1883,10 +1883,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2209,7 +2205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329A5B2C-B2CD-2E4C-9B25-8D30DFCCCE6A}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2472,7 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1F38ED-336F-E241-A27A-3D55AF4798CF}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -2706,7 +2702,7 @@
       <c r="B10" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" t="s">
         <v>94</v>
       </c>
       <c r="D10">
@@ -2729,7 +2725,7 @@
       <c r="B11" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" t="s">
         <v>94</v>
       </c>
       <c r="D11" s="29">
@@ -2752,7 +2748,7 @@
       <c r="B12" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" t="s">
         <v>94</v>
       </c>
       <c r="D12">
@@ -2775,7 +2771,7 @@
       <c r="B13" t="s">
         <v>112</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" t="s">
         <v>94</v>
       </c>
       <c r="D13" s="29">
@@ -2798,7 +2794,7 @@
       <c r="B14" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" t="s">
         <v>187</v>
       </c>
       <c r="E14" t="s">
@@ -2815,7 +2811,7 @@
       <c r="B15" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" t="s">
         <v>187</v>
       </c>
       <c r="E15" t="s">
@@ -2832,7 +2828,7 @@
       <c r="B16" t="s">
         <v>115</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" t="s">
         <v>187</v>
       </c>
       <c r="E16" t="s">
@@ -2849,7 +2845,7 @@
       <c r="B17" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" t="s">
         <v>187</v>
       </c>
       <c r="E17" t="s">
@@ -2869,7 +2865,7 @@
       <c r="B18" t="s">
         <v>117</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" t="s">
         <v>187</v>
       </c>
       <c r="E18" t="s">
@@ -2892,7 +2888,7 @@
       <c r="B19" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" t="s">
         <v>187</v>
       </c>
       <c r="E19" t="s">
@@ -2915,7 +2911,7 @@
       <c r="B20" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" t="s">
         <v>94</v>
       </c>
       <c r="D20">
@@ -2941,7 +2937,7 @@
       <c r="B21" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" t="s">
         <v>187</v>
       </c>
       <c r="E21" t="s">
@@ -2961,7 +2957,7 @@
       <c r="B22" t="s">
         <v>121</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" t="s">
         <v>187</v>
       </c>
       <c r="E22" t="s">
@@ -2981,7 +2977,7 @@
       <c r="B23" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" t="s">
         <v>94</v>
       </c>
       <c r="D23" s="29">
@@ -3007,7 +3003,7 @@
       <c r="B24" t="s">
         <v>123</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" t="s">
         <v>187</v>
       </c>
       <c r="E24" t="s">
@@ -3027,7 +3023,7 @@
       <c r="B25" t="s">
         <v>124</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" t="s">
         <v>187</v>
       </c>
       <c r="E25" t="s">
@@ -3047,7 +3043,7 @@
       <c r="B26" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" t="s">
         <v>187</v>
       </c>
       <c r="E26" t="s">
@@ -3067,7 +3063,7 @@
       <c r="B27" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" t="s">
         <v>187</v>
       </c>
       <c r="E27" t="s">
@@ -3087,7 +3083,7 @@
       <c r="B28" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" t="s">
         <v>187</v>
       </c>
       <c r="E28" t="s">
@@ -3107,7 +3103,7 @@
       <c r="B29" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" t="s">
         <v>187</v>
       </c>
       <c r="E29" t="s">
@@ -3127,7 +3123,7 @@
       <c r="B30" t="s">
         <v>129</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" t="s">
         <v>187</v>
       </c>
       <c r="E30" t="s">
@@ -3147,7 +3143,7 @@
       <c r="B31" t="s">
         <v>130</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" t="s">
         <v>131</v>
       </c>
       <c r="D31">
@@ -3173,7 +3169,7 @@
       <c r="B32" t="s">
         <v>132</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" t="s">
         <v>187</v>
       </c>
       <c r="E32" t="s">
@@ -3193,7 +3189,7 @@
       <c r="B33" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="30" t="s">
         <v>94</v>
       </c>
       <c r="D33" s="30">

</xml_diff>